<commit_message>
feat: Implement core catalog system with admin panel, data management, and supporting utilities, while updating server and removing legacy files.
</commit_message>
<xml_diff>
--- a/database/Samsung_Colores.xlsx
+++ b/database/Samsung_Colores.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -748,20 +748,9 @@
         <v>#b6c0d6</v>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" t="str">
-        <v>c031</v>
-      </c>
-      <c r="B32" t="str">
-        <v>test</v>
-      </c>
-      <c r="C32" t="str">
-        <v>#000000</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C32"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C31"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>